<commit_message>
set 0 m3/h to R20 for survey 1 and R21 for survey 3
</commit_message>
<xml_diff>
--- a/data/surveys.xlsx
+++ b/data/surveys.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/ptrack/case_study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E988A3-29CB-DF4E-9574-ABBDB7C60723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE35407-75FC-474B-BC2C-49FF65093CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="500" windowWidth="21960" windowHeight="13820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7640" yWindow="1020" windowWidth="26300" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$9:$M$9</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$C$9:$M$9</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -712,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:D26"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -965,7 +969,7 @@
         <v>8.4</v>
       </c>
       <c r="F3" s="4">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2">
         <v>319</v>
@@ -1272,7 +1276,7 @@
         <v>207.791666666666</v>
       </c>
       <c r="G5" s="15">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="H5" s="15">
         <v>342.125</v>

</xml_diff>

<commit_message>
modified helper to account for Jalle river only
</commit_message>
<xml_diff>
--- a/data/surveys.xlsx
+++ b/data/surveys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/ptrack/case_study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4F8300-102D-CE4D-B233-AD62B5140939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DBA2BB-BF6F-3547-9379-B039793E95B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="500" windowWidth="20300" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Q_R20</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>∆H</t>
   </si>
 </sst>
 </file>
@@ -396,6 +402,1871 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0299999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5CD7-FD4A-BFAE-F48E7140D878}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="587994048"/>
+        <c:axId val="587799200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="587994048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="587799200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="587799200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="587994048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-1.9499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.4499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.9699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.2000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.0499999999999989</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.7400000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4BAC-8A46-AA90-2356203F6A9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="632117568"/>
+        <c:axId val="632119216"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="632117568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="632119216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="632119216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="632117568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59E21751-8B24-73D1-3CEF-53E0B18E8EBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A7F9B75-1383-435E-833D-BFD76D990E21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -683,10 +2554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV26"/>
+  <dimension ref="A1:AW26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -699,27 +2570,27 @@
     <col min="7" max="7" width="6.33203125" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
     <col min="9" max="9" width="11.83203125" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="15" width="9.1640625" customWidth="1"/>
-    <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="14.5" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" customWidth="1"/>
-    <col min="19" max="19" width="11.1640625" customWidth="1"/>
-    <col min="20" max="20" width="8.1640625" customWidth="1"/>
-    <col min="21" max="21" width="8.83203125" customWidth="1"/>
-    <col min="22" max="22" width="10.6640625" customWidth="1"/>
-    <col min="23" max="38" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="13" max="16" width="9.1640625" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="14.5" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" customWidth="1"/>
+    <col min="20" max="20" width="11.1640625" customWidth="1"/>
+    <col min="21" max="21" width="8.1640625" customWidth="1"/>
+    <col min="22" max="22" width="8.83203125" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" customWidth="1"/>
+    <col min="24" max="39" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -751,118 +2622,121 @@
         <v>7</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="X1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="Y1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AB1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AC1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="AD1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AE1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="AF1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="AG1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AH1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AI1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="10" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="10" t="s">
+      <c r="AK1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="10" t="s">
+      <c r="AL1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="10" t="s">
+      <c r="AM1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="10" t="s">
+      <c r="AN1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="10" t="s">
+      <c r="AO1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="10" t="s">
+      <c r="AP1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="10" t="s">
+      <c r="AQ1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="10" t="s">
+      <c r="AR1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="10" t="s">
+      <c r="AS1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="10" t="s">
+      <c r="AT1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" s="10" t="s">
+      <c r="AU1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" s="10" t="s">
+      <c r="AV1" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -891,90 +2765,94 @@
         <v>373</v>
       </c>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2">
+      <c r="K2" s="2">
+        <f>E2-C2</f>
+        <v>-1.9499999999999993</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2">
         <v>10</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>27</v>
       </c>
-      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
+      <c r="P2" s="2"/>
       <c r="Q2" s="2">
         <v>0</v>
       </c>
       <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
         <v>134.083333333333</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>17.3333333333333</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>0</v>
       </c>
-      <c r="U2" s="3">
+      <c r="V2" s="3">
         <v>47.125</v>
       </c>
-      <c r="V2" s="3">
+      <c r="W2" s="3">
         <v>38.003502626970203</v>
       </c>
-      <c r="W2" s="2"/>
       <c r="X2" s="2"/>
-      <c r="Y2" s="2">
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2">
         <v>9.6525479050336607</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AA2" s="2">
         <v>9.7345191906120672</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AB2" s="2">
         <v>10.196226190476169</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AC2" s="2">
         <v>10.00611607142856</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AD2" s="2">
         <v>9.6121523809523808</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AE2" s="2">
         <v>9.8990526669384202</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AF2" s="2">
         <v>10.26083242884317</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AG2" s="2">
         <v>9.1273125000000022</v>
       </c>
-      <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
-      <c r="AM2" s="2">
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2">
         <v>9.4753547619047627</v>
       </c>
-      <c r="AN2" s="2">
+      <c r="AO2" s="2">
         <v>10.005243452380959</v>
       </c>
-      <c r="AO2" s="2">
+      <c r="AP2" s="2">
         <v>8.3103017857142838</v>
       </c>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="2">
+      <c r="AQ2" s="27"/>
+      <c r="AR2" s="2">
         <v>9.7050535714285733</v>
       </c>
-      <c r="AR2" s="2">
+      <c r="AS2" s="2">
         <v>9.3962125000000007</v>
       </c>
-      <c r="AS2" s="2"/>
       <c r="AT2" s="2"/>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
     </row>
-    <row r="3" spans="1:48" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:49" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1003,25 +2881,26 @@
         <v>208</v>
       </c>
       <c r="J3" s="23"/>
-      <c r="K3" s="23">
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K11" si="0">E3-C3</f>
+        <v>-2.1999999999999993</v>
+      </c>
+      <c r="L3" s="23">
         <v>64</v>
       </c>
-      <c r="L3" s="23">
+      <c r="M3" s="23">
         <v>7</v>
       </c>
-      <c r="M3" s="23">
+      <c r="N3" s="23">
         <v>24</v>
       </c>
-      <c r="N3" s="23"/>
       <c r="O3" s="23"/>
-      <c r="P3" s="23">
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23">
         <v>67.0833333333333</v>
       </c>
-      <c r="Q3" s="23">
+      <c r="R3" s="23">
         <v>61.9583333333333</v>
-      </c>
-      <c r="R3" s="23">
-        <v>0</v>
       </c>
       <c r="S3" s="23">
         <v>0</v>
@@ -1029,76 +2908,79 @@
       <c r="T3" s="23">
         <v>0</v>
       </c>
-      <c r="U3" s="25">
+      <c r="U3" s="23">
+        <v>0</v>
+      </c>
+      <c r="V3" s="25">
         <v>42.6666666666666</v>
       </c>
-      <c r="V3" s="25">
+      <c r="W3" s="25">
         <v>36.525612472160297</v>
       </c>
-      <c r="W3" s="23"/>
       <c r="X3" s="23"/>
-      <c r="Y3" s="23">
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23">
         <v>9.6360678571428569</v>
       </c>
-      <c r="Z3" s="23">
+      <c r="AA3" s="23">
         <v>9.8018660714285719</v>
       </c>
-      <c r="AA3" s="23">
+      <c r="AB3" s="23">
         <v>10.5855869047619</v>
       </c>
-      <c r="AB3" s="23">
+      <c r="AC3" s="23">
         <v>10.33018214285714</v>
       </c>
-      <c r="AC3" s="23">
+      <c r="AD3" s="23">
         <v>9.6485982142857143</v>
       </c>
-      <c r="AD3" s="23">
+      <c r="AE3" s="23">
         <v>9.9715982142857165</v>
       </c>
-      <c r="AE3" s="23">
+      <c r="AF3" s="23">
         <v>10.92704702380953</v>
       </c>
-      <c r="AF3" s="23">
+      <c r="AG3" s="23">
         <v>9.093102380952379</v>
       </c>
-      <c r="AG3" s="23">
+      <c r="AH3" s="23">
         <v>8.6855297619047622</v>
       </c>
-      <c r="AH3" s="23">
+      <c r="AI3" s="23">
         <v>8.9416458333333324</v>
       </c>
-      <c r="AI3" s="23">
+      <c r="AJ3" s="23">
         <v>9.2385910714285728</v>
       </c>
-      <c r="AJ3" s="23">
+      <c r="AK3" s="23">
         <v>9.1267017857142854</v>
       </c>
-      <c r="AK3" s="23">
+      <c r="AL3" s="23">
         <v>9.5699690476190504</v>
       </c>
-      <c r="AL3" s="23">
+      <c r="AM3" s="23">
         <v>9.637910714285713</v>
       </c>
-      <c r="AM3" s="23">
+      <c r="AN3" s="23">
         <v>9.2019785714285707</v>
       </c>
-      <c r="AN3" s="23">
+      <c r="AO3" s="23">
         <v>10.141202380952381</v>
       </c>
-      <c r="AO3" s="23"/>
-      <c r="AP3" s="28"/>
-      <c r="AQ3" s="23">
+      <c r="AP3" s="23"/>
+      <c r="AQ3" s="28"/>
+      <c r="AR3" s="23">
         <v>9.9792398809523792</v>
       </c>
-      <c r="AR3" s="23">
+      <c r="AS3" s="23">
         <v>8.6275785714285718</v>
       </c>
-      <c r="AS3" s="23"/>
       <c r="AT3" s="23"/>
       <c r="AU3" s="23"/>
       <c r="AV3" s="23"/>
+      <c r="AW3" s="23"/>
     </row>
-    <row r="4" spans="1:48" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:49" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -1127,112 +3009,116 @@
         <v>382</v>
       </c>
       <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14">
+      <c r="K4" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.9000000000000004</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14">
         <v>11</v>
       </c>
-      <c r="M4" s="14">
+      <c r="N4" s="14">
         <v>31</v>
       </c>
-      <c r="N4" s="14"/>
       <c r="O4" s="14"/>
-      <c r="P4" s="14">
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14">
         <v>61.2083333333333</v>
       </c>
-      <c r="Q4" s="14">
+      <c r="R4" s="14">
         <v>40.2916666666666</v>
       </c>
-      <c r="R4" s="14">
+      <c r="S4" s="14">
         <v>128.916666666666</v>
       </c>
-      <c r="S4" s="14">
+      <c r="T4" s="14">
         <v>17.75</v>
       </c>
-      <c r="T4" s="14">
+      <c r="U4" s="14">
         <v>0</v>
       </c>
-      <c r="U4" s="16">
+      <c r="V4" s="16">
         <v>35.625</v>
       </c>
-      <c r="V4" s="16">
+      <c r="W4" s="16">
         <v>32.8333333333333</v>
       </c>
-      <c r="W4" s="14">
+      <c r="X4" s="14">
         <v>9.3598885238095253</v>
       </c>
-      <c r="X4" s="14">
+      <c r="Y4" s="14">
         <v>9.9018292023809522</v>
       </c>
-      <c r="Y4" s="14">
+      <c r="Z4" s="14">
         <v>9.608518982142856</v>
       </c>
-      <c r="Z4" s="14">
+      <c r="AA4" s="14">
         <v>9.683357035714284</v>
       </c>
-      <c r="AA4" s="14">
+      <c r="AB4" s="14">
         <v>10.058672625</v>
       </c>
-      <c r="AB4" s="14">
+      <c r="AC4" s="14">
         <v>9.7340520297619015</v>
       </c>
-      <c r="AC4" s="14">
+      <c r="AD4" s="14">
         <v>9.5986493869047642</v>
       </c>
-      <c r="AD4" s="14">
+      <c r="AE4" s="14">
         <v>9.8011417083333345</v>
       </c>
-      <c r="AE4" s="14">
+      <c r="AF4" s="14">
         <v>9.8862252261904757</v>
       </c>
-      <c r="AF4" s="14">
+      <c r="AG4" s="14">
         <v>8.874929767857143</v>
       </c>
-      <c r="AG4" s="14">
+      <c r="AH4" s="14">
         <v>8.6629561904761889</v>
       </c>
-      <c r="AH4" s="14">
+      <c r="AI4" s="14">
         <v>8.8768794761904779</v>
       </c>
-      <c r="AI4" s="14">
+      <c r="AJ4" s="14">
         <v>8.9760425773809516</v>
       </c>
-      <c r="AJ4" s="14">
+      <c r="AK4" s="14">
         <v>8.9377821309523817</v>
       </c>
-      <c r="AK4" s="14">
+      <c r="AL4" s="14">
         <v>9.4961094107142863</v>
       </c>
-      <c r="AL4" s="14">
+      <c r="AM4" s="14">
         <v>9.5524466964285732</v>
       </c>
-      <c r="AM4" s="14">
+      <c r="AN4" s="14">
         <v>9.0938652678571437</v>
       </c>
-      <c r="AN4" s="14">
+      <c r="AO4" s="14">
         <v>10.00374742857144</v>
       </c>
-      <c r="AO4" s="14">
+      <c r="AP4" s="14">
         <v>8.3675158630952389</v>
       </c>
-      <c r="AP4" s="29"/>
-      <c r="AQ4" s="14">
+      <c r="AQ4" s="29"/>
+      <c r="AR4" s="14">
         <v>9.5694240773809529</v>
       </c>
-      <c r="AR4" s="14">
+      <c r="AS4" s="14">
         <v>8.3923471726190488</v>
       </c>
-      <c r="AS4" s="14">
+      <c r="AT4" s="14">
         <v>9.2914157619047621</v>
       </c>
-      <c r="AT4" s="14">
+      <c r="AU4" s="14">
         <v>8.3879609821428591</v>
       </c>
-      <c r="AU4" s="14">
+      <c r="AV4" s="14">
         <v>8.41241548809524</v>
       </c>
-      <c r="AV4" s="14"/>
+      <c r="AW4" s="14"/>
     </row>
-    <row r="5" spans="1:48" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:49" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1261,35 +3147,38 @@
         <v>268</v>
       </c>
       <c r="J5" s="19"/>
-      <c r="K5" s="19">
+      <c r="K5" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.4499999999999993</v>
+      </c>
+      <c r="L5" s="19">
         <v>41</v>
       </c>
-      <c r="L5" s="19"/>
       <c r="M5" s="19"/>
       <c r="N5" s="19"/>
       <c r="O5" s="19"/>
-      <c r="P5" s="19">
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19">
         <v>58.4583333333333</v>
       </c>
-      <c r="Q5" s="19">
+      <c r="R5" s="19">
         <v>60.273972602739697</v>
       </c>
-      <c r="R5" s="19">
+      <c r="S5" s="19">
         <v>121.416666666666</v>
       </c>
-      <c r="S5" s="19">
+      <c r="T5" s="19">
         <v>17.7083333333333</v>
       </c>
-      <c r="T5" s="19">
+      <c r="U5" s="19">
         <v>0</v>
       </c>
-      <c r="U5" s="19">
+      <c r="V5" s="19">
         <v>35.854575846218097</v>
       </c>
-      <c r="V5" s="19">
+      <c r="W5" s="19">
         <v>27.3</v>
       </c>
-      <c r="W5" s="19"/>
       <c r="X5" s="19"/>
       <c r="Y5" s="19"/>
       <c r="Z5" s="19"/>
@@ -1315,8 +3204,9 @@
       <c r="AT5" s="19"/>
       <c r="AU5" s="19"/>
       <c r="AV5" s="19"/>
+      <c r="AW5" s="19"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1346,36 +3236,40 @@
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.9699999999999998</v>
+      </c>
+      <c r="L6" s="2">
         <v>41</v>
       </c>
-      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2">
         <v>57.25</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="R6" s="2">
         <v>46.319663512092497</v>
       </c>
-      <c r="R6" s="2">
+      <c r="S6" s="2">
         <v>116.5</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T6" s="2">
         <v>17.7083333333333</v>
       </c>
-      <c r="T6" s="2">
+      <c r="U6" s="2">
         <v>0</v>
       </c>
-      <c r="U6" s="2">
+      <c r="V6" s="2">
         <v>37.224880382775098</v>
       </c>
-      <c r="V6" s="2">
+      <c r="W6" s="2">
         <v>27.1</v>
       </c>
-      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1404,37 +3298,40 @@
       <c r="J7" s="2">
         <v>0</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2">
+      <c r="K7" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.2000000000000011</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2">
         <v>8</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>38</v>
       </c>
-      <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2">
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2">
         <v>57.7083333333333</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="R7" s="2">
         <v>42.875</v>
       </c>
-      <c r="R7" s="2">
+      <c r="S7" s="2">
         <v>111.68774531181801</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T7" s="2">
         <v>17.559009786989002</v>
       </c>
-      <c r="T7" s="2">
+      <c r="U7" s="2">
         <v>0</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <v>31.625</v>
       </c>
-      <c r="V7" s="2">
+      <c r="W7" s="2">
         <v>26.8175582990397</v>
       </c>
-      <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
@@ -1460,8 +3357,9 @@
       <c r="AT7" s="2"/>
       <c r="AU7" s="2"/>
       <c r="AV7" s="2"/>
+      <c r="AW7" s="2"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1493,19 +3391,20 @@
         <v>0</v>
       </c>
       <c r="K8" s="2">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>-2.0499999999999989</v>
       </c>
       <c r="L8" s="2">
         <v>30</v>
       </c>
       <c r="M8" s="2">
+        <v>30</v>
+      </c>
+      <c r="N8" s="2">
         <v>77</v>
       </c>
-      <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="2">
-        <v>0</v>
-      </c>
+      <c r="P8" s="2"/>
       <c r="Q8" s="2">
         <v>0</v>
       </c>
@@ -1513,18 +3412,20 @@
         <v>0</v>
       </c>
       <c r="S8" s="2">
+        <v>0</v>
+      </c>
+      <c r="T8" s="2">
         <v>17.027600849256899</v>
       </c>
-      <c r="T8" s="2">
+      <c r="U8" s="2">
         <v>0</v>
       </c>
-      <c r="U8" s="2">
+      <c r="V8" s="2">
         <v>47.5</v>
       </c>
-      <c r="V8" s="2">
+      <c r="W8" s="2">
         <v>27.016645326504399</v>
       </c>
-      <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
@@ -1550,8 +3451,9 @@
       <c r="AT8" s="2"/>
       <c r="AU8" s="2"/>
       <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1583,38 +3485,41 @@
         <v>0</v>
       </c>
       <c r="K9" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.5</v>
+      </c>
+      <c r="L9" s="2">
         <v>28</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>6</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>13</v>
       </c>
-      <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="2">
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2">
         <v>65</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>0</v>
       </c>
       <c r="R9" s="2">
         <v>0</v>
       </c>
       <c r="S9" s="2">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
         <v>17</v>
       </c>
-      <c r="T9" s="2">
+      <c r="U9" s="2">
         <v>0</v>
       </c>
-      <c r="U9" s="2">
+      <c r="V9" s="2">
         <v>49.9583333333333</v>
       </c>
-      <c r="V9" s="2">
+      <c r="W9" s="2">
         <v>26.2</v>
       </c>
-      <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
@@ -1640,8 +3545,9 @@
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
       <c r="AV9" s="2"/>
+      <c r="AW9" s="2"/>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1673,17 +3579,18 @@
         <v>0</v>
       </c>
       <c r="K10" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.4000000000000004</v>
+      </c>
+      <c r="L10" s="2">
         <v>24</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>0</v>
       </c>
-      <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="2">
-        <v>0</v>
-      </c>
+      <c r="P10" s="2"/>
       <c r="Q10" s="2">
         <v>0</v>
       </c>
@@ -1691,18 +3598,20 @@
         <v>0</v>
       </c>
       <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
         <v>17.0833333333333</v>
       </c>
-      <c r="T10" s="2">
+      <c r="U10" s="2">
         <v>0</v>
       </c>
-      <c r="U10" s="2">
+      <c r="V10" s="2">
         <v>49.9583333333333</v>
       </c>
-      <c r="V10" s="2">
+      <c r="W10" s="2">
         <v>26.1</v>
       </c>
-      <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
@@ -1728,8 +3637,9 @@
       <c r="AT10" s="2"/>
       <c r="AU10" s="2"/>
       <c r="AV10" s="2"/>
+      <c r="AW10" s="2"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1761,17 +3671,18 @@
         <v>0</v>
       </c>
       <c r="K11" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.7400000000000002</v>
+      </c>
+      <c r="L11" s="2">
         <v>31</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>4</v>
       </c>
-      <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="2">
-        <v>0</v>
-      </c>
+      <c r="P11" s="2"/>
       <c r="Q11" s="2">
         <v>0</v>
       </c>
@@ -1779,20 +3690,23 @@
         <v>0</v>
       </c>
       <c r="S11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
         <v>17.0833333333333</v>
       </c>
-      <c r="T11" s="2">
+      <c r="U11" s="2">
         <v>0</v>
       </c>
-      <c r="U11" s="2">
+      <c r="V11" s="2">
         <v>49.9583333333333</v>
       </c>
-      <c r="V11" s="2">
+      <c r="W11" s="2">
         <v>26.1</v>
       </c>
-      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>99</v>
       </c>
@@ -1815,40 +3729,43 @@
       <c r="G12" s="2">
         <v>250</v>
       </c>
-      <c r="P12" s="2">
-        <f t="shared" ref="P12:V12" si="0">AVERAGE(P2:P11)</f>
+      <c r="Q12" s="2">
+        <f t="shared" ref="Q12:W12" si="1">AVERAGE(Q2:Q11)</f>
         <v>36.67083333333332</v>
       </c>
-      <c r="Q12" s="2">
-        <f t="shared" si="0"/>
+      <c r="R12" s="2">
+        <f t="shared" si="1"/>
         <v>25.171863611483211</v>
       </c>
-      <c r="R12" s="2">
-        <f t="shared" si="0"/>
+      <c r="S12" s="2">
+        <f t="shared" si="1"/>
         <v>61.260441197848294</v>
       </c>
-      <c r="S12" s="2">
-        <f t="shared" si="0"/>
+      <c r="T12" s="2">
+        <f t="shared" si="1"/>
         <v>15.625327730291241</v>
       </c>
-      <c r="T12" s="2">
-        <f t="shared" si="0"/>
+      <c r="U12" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U12" s="2">
-        <f t="shared" si="0"/>
+      <c r="V12" s="2">
+        <f t="shared" si="1"/>
         <v>42.749612289565974</v>
       </c>
-      <c r="V12" s="2">
-        <f t="shared" si="0"/>
+      <c r="W12" s="2">
+        <f t="shared" si="1"/>
         <v>29.39966520580079</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
       <c r="D14" s="2"/>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.2">
@@ -1945,7 +3862,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:O11">
+  <conditionalFormatting sqref="J2:P11">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1982,5 +3899,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated par.xlsx for case 99
</commit_message>
<xml_diff>
--- a/data/surveys.xlsx
+++ b/data/surveys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/ptrack/case_study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DBA2BB-BF6F-3547-9379-B039793E95B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BB40D7-AB16-6345-AF24-DD2FC1482F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2557,7 +2557,7 @@
   <dimension ref="A1:AW26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3714,20 +3714,19 @@
         <v>367</v>
       </c>
       <c r="C12" s="2">
-        <f>AVERAGE(C2:C11)</f>
-        <v>10.709999999999999</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2">
-        <v>8.5</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="G12" s="2">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="2">
         <f t="shared" ref="Q12:W12" si="1">AVERAGE(Q2:Q11)</f>

</xml_diff>

<commit_message>
fixed inconsistant Q_GAL value in surveys
</commit_message>
<xml_diff>
--- a/data/surveys.xlsx
+++ b/data/surveys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/ptrack/case_study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5C5DB9-0850-AD4A-9EAB-2A614ECE4853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8379B37-D390-AA4C-A46B-4297A744D8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="2320" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -689,7 +689,7 @@
   <dimension ref="A1:AW26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1010,7 +1010,7 @@
         <v>573</v>
       </c>
       <c r="I3" s="24">
-        <v>208</v>
+        <v>300</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="2">

</xml_diff>

<commit_message>
new opt with high river level
</commit_message>
<xml_diff>
--- a/data/surveys.xlsx
+++ b/data/surveys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/ptrack/case_study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8379B37-D390-AA4C-A46B-4297A744D8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422D38D6-CC1D-EF4A-A251-5E262AEAAE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -689,7 +689,7 @@
   <dimension ref="A1:AW26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1846,8 +1846,7 @@
         <v>367</v>
       </c>
       <c r="C12" s="2">
-        <f>AVERAGE(C2:C11)</f>
-        <v>10.709999999999999</v>
+        <v>11.45</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>

</xml_diff>